<commit_message>
Optimization - todo update
</commit_message>
<xml_diff>
--- a/data/TH-Inbound-Train-Plan-2025.xlsx
+++ b/data/TH-Inbound-Train-Plan-2025.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler.Dick\Documents\Projects\Education\CEE598RTD\2020\design-project\traffic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qianqiantong/PycharmProjects/yard_design/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5F7F41-D427-0445-876C-0C92AD3B7BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="15" windowWidth="9765" windowHeight="10395"/>
+    <workbookView xWindow="60" yWindow="760" windowWidth="10000" windowHeight="10400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Schedule!$B$1:$C$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -349,7 +363,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -828,7 +842,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -839,7 +853,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -899,9 +912,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -939,9 +952,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -976,7 +989,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1011,7 +1024,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1184,20 +1197,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1208,7 +1221,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -1219,7 +1232,7 @@
         <v>0.11458333333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -1230,7 +1243,7 @@
         <v>0.19791666666666666</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -1241,7 +1254,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -1252,7 +1265,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>104</v>
       </c>
@@ -1263,7 +1276,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -1274,7 +1287,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -1285,7 +1298,7 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -1296,7 +1309,7 @@
         <v>0.35416666666666669</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -1307,7 +1320,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -1318,7 +1331,7 @@
         <v>0.39583333333333331</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1329,7 +1342,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>74</v>
       </c>
@@ -1340,7 +1353,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>75</v>
       </c>
@@ -1351,7 +1364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>76</v>
       </c>
@@ -1362,7 +1375,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>102</v>
       </c>
@@ -1373,7 +1386,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>105</v>
       </c>
@@ -1384,18 +1397,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" t="s">
         <v>85</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -1406,7 +1419,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -1417,7 +1430,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -1428,7 +1441,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -1439,7 +1452,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1450,7 +1463,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -1461,7 +1474,7 @@
         <v>0.94791666666666663</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -1478,19 +1491,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BS44"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="BU5" sqref="BU5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="71" width="9.140625" style="1"/>
+    <col min="1" max="71" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1636,7 +1649,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -1805,7 +1818,7 @@
         <v>0.97916666666666663</v>
       </c>
     </row>
-    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -1974,7 +1987,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>63</v>
       </c>
@@ -2167,7 +2180,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -2313,7 +2326,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -2459,7 +2472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -2605,7 +2618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -2751,7 +2764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -2897,7 +2910,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -3043,7 +3056,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -3189,7 +3202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
@@ -3335,7 +3348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
@@ -3481,7 +3494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
@@ -3627,7 +3640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
@@ -3773,7 +3786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>47</v>
       </c>
@@ -3919,7 +3932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
@@ -4065,7 +4078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
@@ -4205,7 +4218,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
@@ -4345,7 +4358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>53</v>
       </c>
@@ -4479,7 +4492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
@@ -4613,7 +4626,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>61</v>
       </c>
@@ -4747,7 +4760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>62</v>
       </c>
@@ -4881,7 +4894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:71" x14ac:dyDescent="0.2">
       <c r="D24" s="1" t="s">
         <v>40</v>
       </c>
@@ -5009,7 +5022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:71" x14ac:dyDescent="0.2">
       <c r="D25" s="1" t="s">
         <v>41</v>
       </c>
@@ -5131,7 +5144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:71" x14ac:dyDescent="0.2">
       <c r="D26" s="1" t="s">
         <v>42</v>
       </c>
@@ -5253,7 +5266,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:71" x14ac:dyDescent="0.2">
       <c r="D27" s="1" t="s">
         <v>8</v>
       </c>
@@ -5372,7 +5385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:71" x14ac:dyDescent="0.2">
       <c r="D28" s="1" t="s">
         <v>44</v>
       </c>
@@ -5488,7 +5501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:71" x14ac:dyDescent="0.2">
       <c r="D29" s="1" t="s">
         <v>45</v>
       </c>
@@ -5604,7 +5617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:71" x14ac:dyDescent="0.2">
       <c r="D30" s="1" t="s">
         <v>46</v>
       </c>
@@ -5708,7 +5721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:71" x14ac:dyDescent="0.2">
       <c r="D31" s="1" t="s">
         <v>47</v>
       </c>
@@ -5812,7 +5825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:71" x14ac:dyDescent="0.2">
       <c r="D32" s="1" t="s">
         <v>49</v>
       </c>
@@ -5916,7 +5929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="4:68" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:68" x14ac:dyDescent="0.2">
       <c r="D33" s="1" t="s">
         <v>50</v>
       </c>
@@ -6008,7 +6021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="4:68" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:68" x14ac:dyDescent="0.2">
       <c r="D34" s="1" t="s">
         <v>51</v>
       </c>
@@ -6100,7 +6113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="4:68" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:68" x14ac:dyDescent="0.2">
       <c r="D35" s="1" t="s">
         <v>52</v>
       </c>
@@ -6174,7 +6187,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="4:68" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:68" x14ac:dyDescent="0.2">
       <c r="D36" s="1" t="s">
         <v>53</v>
       </c>
@@ -6242,7 +6255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="4:68" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:68" x14ac:dyDescent="0.2">
       <c r="D37" s="1" t="s">
         <v>54</v>
       </c>
@@ -6298,7 +6311,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="4:68" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:68" x14ac:dyDescent="0.2">
       <c r="D38" s="1" t="s">
         <v>55</v>
       </c>
@@ -6342,7 +6355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="4:68" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:68" x14ac:dyDescent="0.2">
       <c r="D39" s="1" t="s">
         <v>56</v>
       </c>
@@ -6386,7 +6399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="4:68" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:68" x14ac:dyDescent="0.2">
       <c r="D40" s="1" t="s">
         <v>58</v>
       </c>
@@ -6424,7 +6437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="4:68" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:68" x14ac:dyDescent="0.2">
       <c r="D41" s="1" t="s">
         <v>59</v>
       </c>
@@ -6450,7 +6463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="4:68" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:68" x14ac:dyDescent="0.2">
       <c r="D42" s="1" t="s">
         <v>60</v>
       </c>
@@ -6464,7 +6477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="4:68" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:68" x14ac:dyDescent="0.2">
       <c r="D43" s="1" t="s">
         <v>61</v>
       </c>
@@ -6472,7 +6485,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="4:68" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:68" x14ac:dyDescent="0.2">
       <c r="D44" s="1" t="s">
         <v>62</v>
       </c>

</xml_diff>